<commit_message>
Added PnP-Sensors model and twin
</commit_message>
<xml_diff>
--- a/sandbox/AzureDigitalTwins/logistics-twin.xlsx
+++ b/sandbox/AzureDigitalTwins/logistics-twin.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/chris_lowndes_avanade_com/Documents/work/avanade/digital, data and AI/offerings/FY21/Industry Solutions/Digital Manufacturing/Avanade Digital Twins/manufacturing simulation/discrete event simulation model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\vscode\industryx-sandbox\industryx\sandbox\AzureDigitalTwins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="314" documentId="8_{4D714356-8071-4450-BEB0-D85022EF2560}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76DFCF67-B496-41AB-A6FC-89B23CF92C10}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80529C7C-8CAE-4C6C-9B30-8FF74FC7302A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1230" windowWidth="18668" windowHeight="20670" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
+    <workbookView xWindow="0" yWindow="1230" windowWidth="18668" windowHeight="20670" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="63">
   <si>
     <t>ModelID</t>
   </si>
@@ -59,121 +59,172 @@
     <t>sim000001</t>
   </si>
   <si>
+    <t>dtmi:isa95:space:Area;1</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:space:ProductionLine;1</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:space:StorageZone;1</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:space:WorkCell;1</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:space:ManufacturingHub;1</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:space:DistributionCenter;3</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:core:LogicalDevice;1</t>
+  </si>
+  <si>
+    <t>COMPANY-B</t>
+  </si>
+  <si>
+    <t>AREA-01</t>
+  </si>
+  <si>
+    <t>AREA-02</t>
+  </si>
+  <si>
+    <t>AREA-03</t>
+  </si>
+  <si>
+    <t>AREA-04</t>
+  </si>
+  <si>
+    <t>AREA-05</t>
+  </si>
+  <si>
+    <t>LINE-1</t>
+  </si>
+  <si>
+    <t>LINE-2</t>
+  </si>
+  <si>
+    <t>LINE-3</t>
+  </si>
+  <si>
+    <t>LINE-4</t>
+  </si>
+  <si>
+    <t>STORAGE-A</t>
+  </si>
+  <si>
+    <t>STORAGE-B</t>
+  </si>
+  <si>
+    <t>STORAGE-C</t>
+  </si>
+  <si>
+    <t>STORAGE-D</t>
+  </si>
+  <si>
+    <t>WORKCELL-1</t>
+  </si>
+  <si>
+    <t>WORKCELL-2</t>
+  </si>
+  <si>
+    <t>HUB-1</t>
+  </si>
+  <si>
+    <t>HUB-2</t>
+  </si>
+  <si>
+    <t>WAREHOUSE-A</t>
+  </si>
+  <si>
+    <t>WAREHOUSE-B</t>
+  </si>
+  <si>
+    <t>WAREHOUSE-C</t>
+  </si>
+  <si>
+    <t>hasPart</t>
+  </si>
+  <si>
+    <t>STORAGE-E</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:asset:Machine;1</t>
+  </si>
+  <si>
+    <t>MACHINE-1</t>
+  </si>
+  <si>
+    <t>MACHINE-2</t>
+  </si>
+  <si>
+    <t>{  "metadata": { "$metadata": {}, "metadataItems": { "Supplier": "Test" } } }</t>
+  </si>
+  <si>
+    <t>locatedIn</t>
+  </si>
+  <si>
+    <t>serves</t>
+  </si>
+  <si>
     <t>dtmi:isa95:agent:Organization;1</t>
   </si>
   <si>
-    <t>dtmi:isa95:space:Area;1</t>
-  </si>
-  <si>
-    <t>dtmi:isa95:space:ProductionLine;1</t>
-  </si>
-  <si>
-    <t>dtmi:isa95:space:StorageZone;1</t>
-  </si>
-  <si>
-    <t>dtmi:isa95:space:WorkCell;1</t>
-  </si>
-  <si>
-    <t>dtmi:isa95:space:ManufacturingHub;1</t>
-  </si>
-  <si>
-    <t>dtmi:isa95:space:DistributionCenter;3</t>
-  </si>
-  <si>
-    <t>dtmi:isa95:core:LogicalDevice;1</t>
-  </si>
-  <si>
     <t>ORG-A</t>
   </si>
   <si>
-    <t>COMPANY-B</t>
-  </si>
-  <si>
-    <t>AREA-01</t>
-  </si>
-  <si>
-    <t>AREA-02</t>
-  </si>
-  <si>
-    <t>AREA-03</t>
-  </si>
-  <si>
-    <t>AREA-04</t>
-  </si>
-  <si>
-    <t>AREA-05</t>
-  </si>
-  <si>
-    <t>LINE-1</t>
-  </si>
-  <si>
-    <t>LINE-2</t>
-  </si>
-  <si>
-    <t>LINE-3</t>
-  </si>
-  <si>
-    <t>LINE-4</t>
-  </si>
-  <si>
-    <t>STORAGE-A</t>
-  </si>
-  <si>
-    <t>STORAGE-B</t>
-  </si>
-  <si>
-    <t>STORAGE-C</t>
-  </si>
-  <si>
-    <t>STORAGE-D</t>
-  </si>
-  <si>
-    <t>WORKCELL-1</t>
-  </si>
-  <si>
-    <t>WORKCELL-2</t>
-  </si>
-  <si>
-    <t>HUB-1</t>
-  </si>
-  <si>
-    <t>HUB-2</t>
-  </si>
-  <si>
-    <t>WAREHOUSE-A</t>
-  </si>
-  <si>
-    <t>WAREHOUSE-B</t>
-  </si>
-  <si>
-    <t>WAREHOUSE-C</t>
-  </si>
-  <si>
-    <t>hasPart</t>
-  </si>
-  <si>
-    <t>STORAGE-E</t>
-  </si>
-  <si>
     <t>dtmi:isa95:agent:Enterprise;1</t>
   </si>
   <si>
-    <t>dtmi:isa95:asset:Machine;1</t>
-  </si>
-  <si>
-    <t>MACHINE-1</t>
-  </si>
-  <si>
-    <t>MACHINE-2</t>
-  </si>
-  <si>
-    <t>{  "metadata": { "$metadata": {}, "metadataItems": { "Supplier": "Test" } } }</t>
-  </si>
-  <si>
-    <t>locatedIn</t>
-  </si>
-  <si>
-    <t>serves</t>
+    <t>DEVICE-1</t>
+  </si>
+  <si>
+    <t>dtmi:isa95:capability:SimulatedSensor;1</t>
+  </si>
+  <si>
+    <t>hosts</t>
+  </si>
+  <si>
+    <t>hasCapability</t>
+  </si>
+  <si>
+    <t>{"Capacity": 12, "Wait": 87.5, "Delay": 190.7, "ArrivalRate": 0.65, "Temperature": 20, "Humidity": 50, "Power": 1500, "Vibration":1, "Uptime":100}</t>
+  </si>
+  <si>
+    <t>DEVICE-2</t>
+  </si>
+  <si>
+    <t>sim000002</t>
+  </si>
+  <si>
+    <t>DEVICE-3</t>
+  </si>
+  <si>
+    <t>sim000003</t>
+  </si>
+  <si>
+    <t>MACHINE-3</t>
+  </si>
+  <si>
+    <t>WORKCELL-3</t>
+  </si>
+  <si>
+    <t>WORKCELL-4</t>
+  </si>
+  <si>
+    <t>MACHINE-4</t>
+  </si>
+  <si>
+    <t>DEVICE-4</t>
+  </si>
+  <si>
+    <t>PnP-Sensors</t>
+  </si>
+  <si>
+    <t>dtmi:azurertos:devkit:gsgmxchip;2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "deviceInformation": { "$metadata": { }, "manufacturer": "MXCHIP" } }    </t>
   </si>
 </sst>
 </file>
@@ -531,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4B3A2-EF53-41B2-9F0F-6F5502ACE162}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -565,21 +616,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -587,13 +638,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -601,13 +652,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -615,13 +666,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -629,13 +680,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -643,13 +694,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -657,288 +708,514 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
         <v>40</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
         <v>41</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" t="s">
         <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
         <v>6</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
-        <v>45</v>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E29" xr:uid="{5093E85F-94E4-4979-9E01-3F5F25EDF789}"/>
+  <autoFilter ref="A1:E36" xr:uid="{5093E85F-94E4-4979-9E01-3F5F25EDF789}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Temperature property to AZ3166 PnP
</commit_message>
<xml_diff>
--- a/sandbox/AzureDigitalTwins/logistics-twin.xlsx
+++ b/sandbox/AzureDigitalTwins/logistics-twin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\vscode\industryx-sandbox\industryx\sandbox\AzureDigitalTwins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80529C7C-8CAE-4C6C-9B30-8FF74FC7302A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487F2A80-0C20-47BD-8B9C-448C50A30DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1230" windowWidth="18668" windowHeight="20670" xr2:uid="{B6154E4F-774F-4730-84F3-5195ADBCD94E}"/>
   </bookViews>
@@ -224,7 +224,7 @@
     <t>dtmi:azurertos:devkit:gsgmxchip;2</t>
   </si>
   <si>
-    <t xml:space="preserve">{ "deviceInformation": { "$metadata": { }, "manufacturer": "MXCHIP" } }    </t>
+    <t xml:space="preserve">{ "HubRegistrationId": "ngfdee342", "Temperature": 0.0, "telemetryInterval": 10, "deviceInformation": { "$metadata": { }, "manufacturer": "MXCHIP" } }    </t>
   </si>
 </sst>
 </file>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E4B3A2-EF53-41B2-9F0F-6F5502ACE162}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>